<commit_message>
Updated figures Added figures as png
</commit_message>
<xml_diff>
--- a/Benchmark_Handbrake.xlsx
+++ b/Benchmark_Handbrake.xlsx
@@ -239,11 +239,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="38665728"/>
-        <c:axId val="105673792"/>
+        <c:axId val="49989120"/>
+        <c:axId val="80987840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38665728"/>
+        <c:axId val="49989120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -253,7 +253,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105673792"/>
+        <c:crossAx val="80987840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -261,7 +261,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105673792"/>
+        <c:axId val="80987840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -291,7 +291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38665728"/>
+        <c:crossAx val="49989120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>
@@ -548,21 +548,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="103163904"/>
-        <c:axId val="102303424"/>
+        <c:axId val="49990144"/>
+        <c:axId val="80990144"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="103163904"/>
+        <c:axId val="49990144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102303424"/>
+        <c:crossAx val="80990144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -570,7 +570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102303424"/>
+        <c:axId val="80990144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -601,7 +601,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103163904"/>
+        <c:crossAx val="49990144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="25"/>

</xml_diff>